<commit_message>
prep for Est & Coasts
changed species ID Juncus gerardii to J. tenuis
</commit_message>
<xml_diff>
--- a/mie_raw-METADATA.xlsx
+++ b/mie_raw-METADATA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slane84\OneDrive - The University Of British Columbia\Documents\Dissertation\HabitatRecovery\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/stefanie_lane_ubc_ca/Documents/Documents/Dissertation/HabitatRecovery/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{6207ADAC-956A-434C-853F-0B893B4CCAB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{6DFDB0AB-DF48-4DE6-B01E-CAE3314E605B}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{6207ADAC-956A-434C-853F-0B893B4CCAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6A974B3-35D6-4796-AC92-30169871A8B6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15120" windowHeight="2240" xr2:uid="{1E31F109-19F3-471F-A751-AC5A7F943C2D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1E31F109-19F3-471F-A751-AC5A7F943C2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
   <si>
     <t>Data table metadata</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>Stefanie Lane</t>
-  </si>
-  <si>
-    <t>visual observation of species presence and abundance</t>
   </si>
   <si>
     <t>Jul. 15-17, 2021</t>
@@ -196,6 +193,12 @@
   </si>
   <si>
     <t xml:space="preserve">species codes derived from first two letters of genus, first two letters of species. 'bare' signifies no above-ground cover within the plot, calcualted as 100-(sum of species cover abundance). Please see accompanying file 'species.xlsx' for full list of species codes and corresponding nomenclature. </t>
+  </si>
+  <si>
+    <t>visual observation of species presence and abundance in above-ground vegetation</t>
+  </si>
+  <si>
+    <t>ere (Englishman River Estuary, not included in analysis), lqre (Little Qualicum River Estuary), nre (Nanaimo River Estuary)</t>
   </si>
 </sst>
 </file>
@@ -300,7 +303,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -635,21 +638,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF7BC7A-DB3B-40A8-AB2C-CF64F213BB7A}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
-    <col min="4" max="4" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.26953125" customWidth="1"/>
-    <col min="6" max="6" width="50.36328125" customWidth="1"/>
+    <col min="4" max="4" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" customWidth="1"/>
+    <col min="6" max="6" width="50.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -659,7 +662,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -671,7 +674,7 @@
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -683,7 +686,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
@@ -695,7 +698,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -707,19 +710,19 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -731,31 +734,31 @@
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
     </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -765,7 +768,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
@@ -775,7 +778,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>11</v>
       </c>
@@ -795,117 +798,119 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" s="2" customFormat="1" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:7" s="2" customFormat="1" ht="36.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="10" t="s">
+      <c r="B14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="G14"/>
+    </row>
+    <row r="15" spans="1:7" s="2" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="1:7" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="10"/>
-      <c r="G13"/>
-    </row>
-    <row r="14" spans="1:7" s="2" customFormat="1" ht="35.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14"/>
-    </row>
-    <row r="15" spans="1:7" s="2" customFormat="1" ht="104.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="10" t="s">
+      <c r="D16" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="1:6" ht="48.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="84.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>48</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15"/>
-    </row>
-    <row r="16" spans="1:7" s="2" customFormat="1" ht="61" x14ac:dyDescent="0.35">
-      <c r="A16" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16"/>
-    </row>
-    <row r="17" spans="1:6" ht="47" x14ac:dyDescent="0.35">
-      <c r="A17" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="81.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>49</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
@@ -923,18 +928,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1167,6 +1172,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5947985-95F5-4280-98D1-2F72C01BC72D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A387D7E-E89D-465E-AC59-E89ECF806315}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -1179,14 +1192,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="360018dd-41eb-4458-b1d4-4b46a95a2b02"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5947985-95F5-4280-98D1-2F72C01BC72D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>